<commit_message>
adjust panel order in fig2 and fig4
</commit_message>
<xml_diff>
--- a/outcome/fig2.xlsx
+++ b/outcome/fig2.xlsx
@@ -57,16 +57,16 @@
     <t xml:space="preserve">1990</t>
   </si>
   <si>
+    <t xml:space="preserve">2019</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diff1</t>
   </si>
   <si>
-    <t xml:space="preserve">2019</t>
+    <t xml:space="preserve">2021</t>
   </si>
   <si>
     <t xml:space="preserve">Diff2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021</t>
   </si>
   <si>
     <t xml:space="preserve">ASM</t>
@@ -5477,10 +5477,10 @@
         <v>1.34166666666667</v>
       </c>
       <c r="D2" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.408333333333333</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1.75</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -5496,10 +5496,10 @@
         <v>1.54166666666667</v>
       </c>
       <c r="D3" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.0666666666666667</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.60833333333333</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -5515,16 +5515,16 @@
         <v>1.4</v>
       </c>
       <c r="D4" t="n">
+        <v>1.46666666666667</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0666666666666667</v>
       </c>
-      <c r="E4" t="n">
-        <v>1.46666666666667</v>
-      </c>
       <c r="F4" t="n">
+        <v>1.50833333333333</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.50833333333333</v>
       </c>
     </row>
     <row r="5">
@@ -5538,16 +5538,16 @@
         <v>1.53333333333333</v>
       </c>
       <c r="D5" t="n">
+        <v>1.66666666666667</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.133333333333334</v>
       </c>
-      <c r="E5" t="n">
-        <v>1.66666666666667</v>
-      </c>
       <c r="F5" t="n">
+        <v>1.74166666666667</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.208333333333333</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.74166666666667</v>
       </c>
     </row>
     <row r="6">
@@ -5561,16 +5561,16 @@
         <v>1.55</v>
       </c>
       <c r="D6" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E6" t="n">
-        <v>1.59166666666667</v>
-      </c>
       <c r="F6" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.0666666666666664</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.61666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -5584,10 +5584,10 @@
         <v>1.53333333333333</v>
       </c>
       <c r="D7" t="n">
+        <v>1.69166666666667</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1.69166666666667</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
@@ -5603,10 +5603,10 @@
         <v>1.45</v>
       </c>
       <c r="D8" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.125</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.575</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -5622,10 +5622,10 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D9" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="E9" t="n">
         <v>0.166666666666667</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1.675</v>
       </c>
       <c r="F9"/>
       <c r="G9"/>
@@ -5641,16 +5641,16 @@
         <v>1.43333333333333</v>
       </c>
       <c r="D10" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>1.525</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>0.0916666666666668</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1.525</v>
       </c>
     </row>
     <row r="11">
@@ -5664,16 +5664,16 @@
         <v>1.6</v>
       </c>
       <c r="D11" t="n">
+        <v>1.69166666666667</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E11" t="n">
-        <v>1.69166666666667</v>
-      </c>
       <c r="F11" t="n">
+        <v>1.70833333333333</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1.70833333333333</v>
       </c>
     </row>
     <row r="12">
@@ -5687,10 +5687,10 @@
         <v>1.46666666666667</v>
       </c>
       <c r="D12" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.116666666666666</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1.58333333333333</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -5706,16 +5706,16 @@
         <v>1.325</v>
       </c>
       <c r="D13" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.0249999999999999</v>
       </c>
-      <c r="E13" t="n">
-        <v>1.35</v>
-      </c>
       <c r="F13" t="n">
+        <v>1.35833333333333</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.0333333333333334</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1.35833333333333</v>
       </c>
     </row>
     <row r="14">
@@ -5729,16 +5729,16 @@
         <v>1.525</v>
       </c>
       <c r="D14" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="E14" t="n">
         <v>0.116666666666666</v>
       </c>
-      <c r="E14" t="n">
-        <v>1.64166666666667</v>
-      </c>
       <c r="F14" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.125</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1.65</v>
       </c>
     </row>
     <row r="15">
@@ -5752,16 +5752,16 @@
         <v>1.30833333333333</v>
       </c>
       <c r="D15" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E15" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E15" t="n">
-        <v>1.4</v>
-      </c>
       <c r="F15" t="n">
+        <v>1.41666666666667</v>
+      </c>
+      <c r="G15" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1.41666666666667</v>
       </c>
     </row>
     <row r="16">
@@ -5775,10 +5775,10 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D16" t="n">
+        <v>1.80833333333333</v>
+      </c>
+      <c r="E16" t="n">
         <v>0.366666666666667</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1.80833333333333</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -5794,10 +5794,10 @@
         <v>1.525</v>
       </c>
       <c r="D17" t="n">
+        <v>1.75833333333333</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.233333333333333</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1.75833333333333</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -5813,10 +5813,10 @@
         <v>1.53333333333333</v>
       </c>
       <c r="D18" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="E18" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1.64166666666667</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -5832,16 +5832,16 @@
         <v>1.60833333333333</v>
       </c>
       <c r="D19" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E19" t="n">
         <v>-0.0333333333333334</v>
       </c>
-      <c r="E19" t="n">
-        <v>1.575</v>
-      </c>
       <c r="F19" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="G19" t="n">
         <v>0.00833333333333308</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1.61666666666667</v>
       </c>
     </row>
     <row r="20">
@@ -5855,16 +5855,16 @@
         <v>1.36666666666667</v>
       </c>
       <c r="D20" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E20" t="n">
         <v>0.233333333333333</v>
       </c>
-      <c r="E20" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F20" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="G20" t="n">
         <v>0.258333333333334</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1.625</v>
       </c>
     </row>
     <row r="21">
@@ -5878,16 +5878,16 @@
         <v>1.41666666666667</v>
       </c>
       <c r="D21" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E21" t="n">
         <v>0.125</v>
       </c>
-      <c r="E21" t="n">
-        <v>1.54166666666667</v>
-      </c>
       <c r="F21" t="n">
+        <v>1.55833333333333</v>
+      </c>
+      <c r="G21" t="n">
         <v>0.141666666666667</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1.55833333333333</v>
       </c>
     </row>
     <row r="22">
@@ -5901,16 +5901,16 @@
         <v>1.29166666666667</v>
       </c>
       <c r="D22" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="E22" t="n">
         <v>0.15</v>
       </c>
-      <c r="E22" t="n">
-        <v>1.44166666666667</v>
-      </c>
       <c r="F22" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="G22" t="n">
         <v>0.133333333333333</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1.425</v>
       </c>
     </row>
     <row r="23">
@@ -5924,16 +5924,16 @@
         <v>1.30833333333333</v>
       </c>
       <c r="D23" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E23" t="n">
-        <v>1.45</v>
-      </c>
       <c r="F23" t="n">
+        <v>1.46666666666667</v>
+      </c>
+      <c r="G23" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1.46666666666667</v>
       </c>
     </row>
     <row r="24">
@@ -5947,16 +5947,16 @@
         <v>1.55</v>
       </c>
       <c r="D24" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.0583333333333333</v>
       </c>
-      <c r="E24" t="n">
-        <v>1.60833333333333</v>
-      </c>
       <c r="F24" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="G24" t="n">
         <v>0.0666666666666664</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1.61666666666667</v>
       </c>
     </row>
     <row r="25">
@@ -5970,16 +5970,16 @@
         <v>1.4</v>
       </c>
       <c r="D25" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.0916666666666663</v>
       </c>
-      <c r="E25" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F25" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G25" t="n">
         <v>0.0999999999999999</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1.5</v>
       </c>
     </row>
     <row r="26">
@@ -5993,16 +5993,16 @@
         <v>1.525</v>
       </c>
       <c r="D26" t="n">
+        <v>1.70833333333333</v>
+      </c>
+      <c r="E26" t="n">
         <v>0.183333333333333</v>
       </c>
-      <c r="E26" t="n">
-        <v>1.70833333333333</v>
-      </c>
       <c r="F26" t="n">
+        <v>1.725</v>
+      </c>
+      <c r="G26" t="n">
         <v>0.2</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1.725</v>
       </c>
     </row>
     <row r="27">
@@ -6016,16 +6016,16 @@
         <v>1.31666666666667</v>
       </c>
       <c r="D27" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="E27" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>1.425</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1.425</v>
       </c>
     </row>
     <row r="28">
@@ -6039,16 +6039,16 @@
         <v>1.35</v>
       </c>
       <c r="D28" t="n">
+        <v>1.50833333333333</v>
+      </c>
+      <c r="E28" t="n">
         <v>0.158333333333334</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>1.50833333333333</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>0.158333333333334</v>
-      </c>
-      <c r="G28" t="n">
-        <v>1.50833333333333</v>
       </c>
     </row>
     <row r="29">
@@ -6062,16 +6062,16 @@
         <v>1.575</v>
       </c>
       <c r="D29" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E29" t="n">
         <v>0.0249999999999999</v>
       </c>
-      <c r="E29" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F29" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="G29" t="n">
         <v>0.0416666666666665</v>
-      </c>
-      <c r="G29" t="n">
-        <v>1.61666666666667</v>
       </c>
     </row>
     <row r="30">
@@ -6085,16 +6085,16 @@
         <v>1.26666666666667</v>
       </c>
       <c r="D30" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E30" t="n">
         <v>0.133333333333334</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>1.4</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>0.133333333333334</v>
-      </c>
-      <c r="G30" t="n">
-        <v>1.4</v>
       </c>
     </row>
     <row r="31">
@@ -6108,16 +6108,16 @@
         <v>1.31666666666667</v>
       </c>
       <c r="D31" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E31" t="n">
         <v>0.0333333333333332</v>
       </c>
-      <c r="E31" t="n">
-        <v>1.35</v>
-      </c>
       <c r="F31" t="n">
+        <v>1.35833333333333</v>
+      </c>
+      <c r="G31" t="n">
         <v>0.0416666666666667</v>
-      </c>
-      <c r="G31" t="n">
-        <v>1.35833333333333</v>
       </c>
     </row>
     <row r="32">
@@ -6131,16 +6131,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D32" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="E32" t="n">
         <v>0.0749999999999997</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>1.58333333333333</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>0.0749999999999997</v>
-      </c>
-      <c r="G32" t="n">
-        <v>1.58333333333333</v>
       </c>
     </row>
     <row r="33">
@@ -6154,16 +6154,16 @@
         <v>1.58333333333333</v>
       </c>
       <c r="D33" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="E33" t="n">
         <v>-0.0666666666666667</v>
       </c>
-      <c r="E33" t="n">
-        <v>1.51666666666667</v>
-      </c>
       <c r="F33" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="G33" t="n">
         <v>-0.0416666666666665</v>
-      </c>
-      <c r="G33" t="n">
-        <v>1.54166666666667</v>
       </c>
     </row>
     <row r="34">
@@ -6177,16 +6177,16 @@
         <v>1.58333333333333</v>
       </c>
       <c r="D34" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E34" t="n">
         <v>0.0500000000000003</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>1.63333333333333</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>0.0500000000000003</v>
-      </c>
-      <c r="G34" t="n">
-        <v>1.63333333333333</v>
       </c>
     </row>
     <row r="35">
@@ -6200,16 +6200,16 @@
         <v>1.38333333333333</v>
       </c>
       <c r="D35" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="E35" t="n">
         <v>0.133333333333333</v>
       </c>
-      <c r="E35" t="n">
-        <v>1.51666666666667</v>
-      </c>
       <c r="F35" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="G35" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G35" t="n">
-        <v>1.53333333333333</v>
       </c>
     </row>
     <row r="36">
@@ -6223,16 +6223,16 @@
         <v>1.6</v>
       </c>
       <c r="D36" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E36" t="n">
         <v>0</v>
       </c>
-      <c r="E36" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F36" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="G36" t="n">
         <v>0.0416666666666667</v>
-      </c>
-      <c r="G36" t="n">
-        <v>1.64166666666667</v>
       </c>
     </row>
     <row r="37">
@@ -6246,10 +6246,10 @@
         <v>1.49166666666667</v>
       </c>
       <c r="D37" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="E37" t="n">
         <v>0.125</v>
-      </c>
-      <c r="E37" t="n">
-        <v>1.61666666666667</v>
       </c>
       <c r="F37"/>
       <c r="G37"/>
@@ -6265,10 +6265,10 @@
         <v>1.425</v>
       </c>
       <c r="D38" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="E38" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="E38" t="n">
-        <v>1.53333333333333</v>
       </c>
       <c r="F38"/>
       <c r="G38"/>
@@ -6284,10 +6284,10 @@
         <v>1.48333333333333</v>
       </c>
       <c r="D39" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E39" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="E39" t="n">
-        <v>1.59166666666667</v>
       </c>
       <c r="F39"/>
       <c r="G39"/>
@@ -6303,10 +6303,10 @@
         <v>1.35833333333333</v>
       </c>
       <c r="D40" t="n">
+        <v>1.475</v>
+      </c>
+      <c r="E40" t="n">
         <v>0.116666666666666</v>
-      </c>
-      <c r="E40" t="n">
-        <v>1.475</v>
       </c>
       <c r="F40"/>
       <c r="G40"/>
@@ -6322,16 +6322,16 @@
         <v>1.41666666666667</v>
       </c>
       <c r="D41" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E41" t="n">
         <v>0.175</v>
       </c>
-      <c r="E41" t="n">
-        <v>1.59166666666667</v>
-      </c>
       <c r="F41" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="G41" t="n">
         <v>0.191666666666667</v>
-      </c>
-      <c r="G41" t="n">
-        <v>1.60833333333333</v>
       </c>
     </row>
     <row r="42">
@@ -6345,10 +6345,10 @@
         <v>1.73333333333333</v>
       </c>
       <c r="D42" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="E42" t="n">
         <v>-0.0750000000000002</v>
-      </c>
-      <c r="E42" t="n">
-        <v>1.65833333333333</v>
       </c>
       <c r="F42"/>
       <c r="G42"/>
@@ -6364,16 +6364,16 @@
         <v>1.6</v>
       </c>
       <c r="D43" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E43" t="n">
         <v>0</v>
       </c>
-      <c r="E43" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F43" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="G43" t="n">
         <v>0.00833333333333353</v>
-      </c>
-      <c r="G43" t="n">
-        <v>1.60833333333333</v>
       </c>
     </row>
     <row r="44">
@@ -6387,16 +6387,16 @@
         <v>1.39166666666667</v>
       </c>
       <c r="D44" t="n">
+        <v>1.38333333333333</v>
+      </c>
+      <c r="E44" t="n">
         <v>-0.00833333333333308</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>1.38333333333333</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>-0.00833333333333308</v>
-      </c>
-      <c r="G44" t="n">
-        <v>1.38333333333333</v>
       </c>
     </row>
     <row r="45">
@@ -6410,16 +6410,16 @@
         <v>1.43333333333333</v>
       </c>
       <c r="D45" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="E45" t="n">
         <v>0.0083333333333333</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>1.44166666666667</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>0.0083333333333333</v>
-      </c>
-      <c r="G45" t="n">
-        <v>1.44166666666667</v>
       </c>
     </row>
     <row r="46">
@@ -6433,16 +6433,16 @@
         <v>1.65833333333333</v>
       </c>
       <c r="D46" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="E46" t="n">
         <v>-0.00833333333333308</v>
       </c>
-      <c r="E46" t="n">
-        <v>1.65</v>
-      </c>
       <c r="F46" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="G46" t="n">
         <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>1.65833333333333</v>
       </c>
     </row>
     <row r="47">
@@ -6456,16 +6456,16 @@
         <v>1.29166666666667</v>
       </c>
       <c r="D47" t="n">
+        <v>1.39166666666667</v>
+      </c>
+      <c r="E47" t="n">
         <v>0.0999999999999999</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>1.39166666666667</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>0.0999999999999999</v>
-      </c>
-      <c r="G47" t="n">
-        <v>1.39166666666667</v>
       </c>
     </row>
     <row r="48">
@@ -6479,16 +6479,16 @@
         <v>1.61666666666667</v>
       </c>
       <c r="D48" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E48" t="n">
         <v>0.0166666666666671</v>
       </c>
-      <c r="E48" t="n">
-        <v>1.63333333333333</v>
-      </c>
       <c r="F48" t="n">
+        <v>1.725</v>
+      </c>
+      <c r="G48" t="n">
         <v>0.108333333333334</v>
-      </c>
-      <c r="G48" t="n">
-        <v>1.725</v>
       </c>
     </row>
     <row r="49">
@@ -6502,16 +6502,16 @@
         <v>1.35</v>
       </c>
       <c r="D49" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="E49" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E49" t="n">
-        <v>1.45833333333333</v>
-      </c>
       <c r="F49" t="n">
+        <v>1.48333333333333</v>
+      </c>
+      <c r="G49" t="n">
         <v>0.133333333333334</v>
-      </c>
-      <c r="G49" t="n">
-        <v>1.48333333333333</v>
       </c>
     </row>
     <row r="50">
@@ -6525,16 +6525,16 @@
         <v>1.4</v>
       </c>
       <c r="D50" t="n">
+        <v>1.475</v>
+      </c>
+      <c r="E50" t="n">
         <v>0.0749999999999997</v>
       </c>
-      <c r="E50" t="n">
-        <v>1.475</v>
-      </c>
       <c r="F50" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="G50" t="n">
         <v>0.0916666666666663</v>
-      </c>
-      <c r="G50" t="n">
-        <v>1.49166666666667</v>
       </c>
     </row>
     <row r="51">
@@ -6548,16 +6548,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D51" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="E51" t="n">
         <v>0.15</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>1.65833333333333</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G51" t="n">
-        <v>1.65833333333333</v>
       </c>
     </row>
     <row r="52">
@@ -6571,16 +6571,16 @@
         <v>1.70833333333333</v>
       </c>
       <c r="D52" t="n">
+        <v>1.71666666666667</v>
+      </c>
+      <c r="E52" t="n">
         <v>0.00833333333333353</v>
       </c>
-      <c r="E52" t="n">
-        <v>1.71666666666667</v>
-      </c>
       <c r="F52" t="n">
+        <v>1.725</v>
+      </c>
+      <c r="G52" t="n">
         <v>0.0166666666666671</v>
-      </c>
-      <c r="G52" t="n">
-        <v>1.725</v>
       </c>
     </row>
     <row r="53">
@@ -6594,16 +6594,16 @@
         <v>1.43333333333333</v>
       </c>
       <c r="D53" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E53" t="n">
         <v>0.2</v>
       </c>
-      <c r="E53" t="n">
-        <v>1.63333333333333</v>
-      </c>
       <c r="F53" t="n">
+        <v>1.66666666666667</v>
+      </c>
+      <c r="G53" t="n">
         <v>0.233333333333333</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1.66666666666667</v>
       </c>
     </row>
     <row r="54">
@@ -6617,16 +6617,16 @@
         <v>1.54166666666667</v>
       </c>
       <c r="D54" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E54" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E54" t="n">
-        <v>1.63333333333333</v>
-      </c>
       <c r="F54" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="G54" t="n">
         <v>0.0999999999999999</v>
-      </c>
-      <c r="G54" t="n">
-        <v>1.64166666666667</v>
       </c>
     </row>
     <row r="55">
@@ -6640,16 +6640,16 @@
         <v>1.39166666666667</v>
       </c>
       <c r="D55" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E55" t="n">
         <v>0.15</v>
       </c>
-      <c r="E55" t="n">
-        <v>1.54166666666667</v>
-      </c>
       <c r="F55" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="G55" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G55" t="n">
-        <v>1.55</v>
       </c>
     </row>
     <row r="56">
@@ -6663,16 +6663,16 @@
         <v>1.36666666666667</v>
       </c>
       <c r="D56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E56" t="n">
         <v>0.133333333333334</v>
       </c>
-      <c r="E56" t="n">
-        <v>1.5</v>
-      </c>
       <c r="F56" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="G56" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G56" t="n">
-        <v>1.51666666666667</v>
       </c>
     </row>
     <row r="57">
@@ -6686,16 +6686,16 @@
         <v>1.5</v>
       </c>
       <c r="D57" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E57" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E57" t="n">
-        <v>1.59166666666667</v>
-      </c>
       <c r="F57" t="n">
+        <v>1.56666666666667</v>
+      </c>
+      <c r="G57" t="n">
         <v>0.0666666666666667</v>
-      </c>
-      <c r="G57" t="n">
-        <v>1.56666666666667</v>
       </c>
     </row>
     <row r="58">
@@ -6709,16 +6709,16 @@
         <v>1.40833333333333</v>
       </c>
       <c r="D58" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E58" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="E58" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F58" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G58" t="n">
         <v>0.0916666666666668</v>
-      </c>
-      <c r="G58" t="n">
-        <v>1.5</v>
       </c>
     </row>
     <row r="59">
@@ -6732,16 +6732,16 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D59" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="E59" t="n">
         <v>0.0916666666666666</v>
       </c>
-      <c r="E59" t="n">
-        <v>1.53333333333333</v>
-      </c>
       <c r="F59" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="G59" t="n">
         <v>0.1</v>
-      </c>
-      <c r="G59" t="n">
-        <v>1.54166666666667</v>
       </c>
     </row>
     <row r="60">
@@ -6755,16 +6755,16 @@
         <v>1.425</v>
       </c>
       <c r="D60" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="E60" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E60" t="n">
-        <v>1.53333333333333</v>
-      </c>
       <c r="F60" t="n">
+        <v>1.55833333333333</v>
+      </c>
+      <c r="G60" t="n">
         <v>0.133333333333333</v>
-      </c>
-      <c r="G60" t="n">
-        <v>1.55833333333333</v>
       </c>
     </row>
     <row r="61">
@@ -6778,16 +6778,16 @@
         <v>1.46666666666667</v>
       </c>
       <c r="D61" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="E61" t="n">
         <v>0.191666666666666</v>
       </c>
-      <c r="E61" t="n">
-        <v>1.65833333333333</v>
-      </c>
       <c r="F61" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="G61" t="n">
         <v>0.166666666666667</v>
-      </c>
-      <c r="G61" t="n">
-        <v>1.63333333333333</v>
       </c>
     </row>
     <row r="62">
@@ -6801,16 +6801,16 @@
         <v>1.45833333333333</v>
       </c>
       <c r="D62" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E62" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E62" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F62" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="G62" t="n">
         <v>0.175</v>
-      </c>
-      <c r="G62" t="n">
-        <v>1.63333333333333</v>
       </c>
     </row>
     <row r="63">
@@ -6824,16 +6824,16 @@
         <v>1.70833333333333</v>
       </c>
       <c r="D63" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="E63" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E63" t="n">
-        <v>1.75</v>
-      </c>
       <c r="F63" t="n">
+        <v>1.76666666666667</v>
+      </c>
+      <c r="G63" t="n">
         <v>0.0583333333333336</v>
-      </c>
-      <c r="G63" t="n">
-        <v>1.76666666666667</v>
       </c>
     </row>
     <row r="64">
@@ -6847,16 +6847,16 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D64" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E64" t="n">
         <v>0.158333333333333</v>
       </c>
-      <c r="E64" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F64" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="G64" t="n">
         <v>0.166666666666667</v>
-      </c>
-      <c r="G64" t="n">
-        <v>1.60833333333333</v>
       </c>
     </row>
     <row r="65">
@@ -6870,16 +6870,16 @@
         <v>1.575</v>
       </c>
       <c r="D65" t="n">
+        <v>1.71666666666667</v>
+      </c>
+      <c r="E65" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E65" t="n">
-        <v>1.71666666666667</v>
-      </c>
       <c r="F65" t="n">
+        <v>1.725</v>
+      </c>
+      <c r="G65" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G65" t="n">
-        <v>1.725</v>
       </c>
     </row>
     <row r="66">
@@ -6893,10 +6893,10 @@
         <v>1.425</v>
       </c>
       <c r="D66" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="E66" t="n">
         <v>0.0166666666666666</v>
-      </c>
-      <c r="E66" t="n">
-        <v>1.44166666666667</v>
       </c>
       <c r="F66"/>
       <c r="G66"/>
@@ -6912,16 +6912,16 @@
         <v>1.525</v>
       </c>
       <c r="D67" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="E67" t="n">
         <v>0.0916666666666663</v>
       </c>
-      <c r="E67" t="n">
-        <v>1.61666666666667</v>
-      </c>
       <c r="F67" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="G67" t="n">
         <v>0.0499999999999998</v>
-      </c>
-      <c r="G67" t="n">
-        <v>1.575</v>
       </c>
     </row>
     <row r="68">
@@ -6935,16 +6935,16 @@
         <v>1.45833333333333</v>
       </c>
       <c r="D68" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E68" t="n">
         <v>0.0333333333333332</v>
       </c>
-      <c r="E68" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F68" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="G68" t="n">
         <v>0.075</v>
-      </c>
-      <c r="G68" t="n">
-        <v>1.53333333333333</v>
       </c>
     </row>
     <row r="69">
@@ -6958,16 +6958,16 @@
         <v>1.35833333333333</v>
       </c>
       <c r="D69" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E69" t="n">
         <v>0.0916666666666666</v>
       </c>
-      <c r="E69" t="n">
-        <v>1.45</v>
-      </c>
       <c r="F69" t="n">
+        <v>1.46666666666667</v>
+      </c>
+      <c r="G69" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G69" t="n">
-        <v>1.46666666666667</v>
       </c>
     </row>
     <row r="70">
@@ -6981,16 +6981,16 @@
         <v>1.41666666666667</v>
       </c>
       <c r="D70" t="n">
+        <v>1.55833333333333</v>
+      </c>
+      <c r="E70" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E70" t="n">
-        <v>1.55833333333333</v>
-      </c>
       <c r="F70" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="G70" t="n">
         <v>0.175</v>
-      </c>
-      <c r="G70" t="n">
-        <v>1.59166666666667</v>
       </c>
     </row>
     <row r="71">
@@ -7004,16 +7004,16 @@
         <v>1.46666666666667</v>
       </c>
       <c r="D71" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E71" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E71" t="n">
-        <v>1.575</v>
-      </c>
       <c r="F71" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="G71" t="n">
         <v>0.125</v>
-      </c>
-      <c r="G71" t="n">
-        <v>1.59166666666667</v>
       </c>
     </row>
     <row r="72">
@@ -7027,16 +7027,16 @@
         <v>1.43333333333333</v>
       </c>
       <c r="D72" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E72" t="n">
         <v>0.0583333333333331</v>
       </c>
-      <c r="E72" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F72" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="G72" t="n">
         <v>0.0999999999999999</v>
-      </c>
-      <c r="G72" t="n">
-        <v>1.53333333333333</v>
       </c>
     </row>
     <row r="73">
@@ -7050,16 +7050,16 @@
         <v>1.60833333333333</v>
       </c>
       <c r="D73" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="E73" t="n">
         <v>-0.0250000000000001</v>
       </c>
-      <c r="E73" t="n">
-        <v>1.58333333333333</v>
-      </c>
       <c r="F73" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G73" t="n">
         <v>-0.00833333333333353</v>
-      </c>
-      <c r="G73" t="n">
-        <v>1.6</v>
       </c>
     </row>
     <row r="74">
@@ -7073,16 +7073,16 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D74" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E74" t="n">
         <v>0.133333333333333</v>
       </c>
-      <c r="E74" t="n">
-        <v>1.575</v>
-      </c>
       <c r="F74" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="G74" t="n">
         <v>0.141666666666667</v>
-      </c>
-      <c r="G74" t="n">
-        <v>1.58333333333333</v>
       </c>
     </row>
     <row r="75">
@@ -7096,16 +7096,16 @@
         <v>1.575</v>
       </c>
       <c r="D75" t="n">
+        <v>1.66666666666667</v>
+      </c>
+      <c r="E75" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E75" t="n">
-        <v>1.66666666666667</v>
-      </c>
       <c r="F75" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G75" t="n">
         <v>0.125</v>
-      </c>
-      <c r="G75" t="n">
-        <v>1.7</v>
       </c>
     </row>
     <row r="76">
@@ -7119,10 +7119,10 @@
         <v>1.3</v>
       </c>
       <c r="D76" t="n">
+        <v>1.66666666666667</v>
+      </c>
+      <c r="E76" t="n">
         <v>0.366666666666667</v>
-      </c>
-      <c r="E76" t="n">
-        <v>1.66666666666667</v>
       </c>
       <c r="F76"/>
       <c r="G76"/>
@@ -7138,16 +7138,16 @@
         <v>1.36666666666667</v>
       </c>
       <c r="D77" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="E77" t="n">
         <v>0.166666666666667</v>
       </c>
-      <c r="E77" t="n">
-        <v>1.53333333333333</v>
-      </c>
       <c r="F77" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="G77" t="n">
         <v>0.183333333333334</v>
-      </c>
-      <c r="G77" t="n">
-        <v>1.55</v>
       </c>
     </row>
     <row r="78">
@@ -7161,16 +7161,16 @@
         <v>1.5</v>
       </c>
       <c r="D78" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E78" t="n">
         <v>-0.00833333333333353</v>
       </c>
-      <c r="E78" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F78" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="G78" t="n">
         <v>0.0416666666666667</v>
-      </c>
-      <c r="G78" t="n">
-        <v>1.54166666666667</v>
       </c>
     </row>
     <row r="79">
@@ -7184,16 +7184,16 @@
         <v>1.40833333333333</v>
       </c>
       <c r="D79" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="E79" t="n">
         <v>0.175</v>
       </c>
-      <c r="E79" t="n">
-        <v>1.58333333333333</v>
-      </c>
       <c r="F79" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="G79" t="n">
         <v>0.183333333333334</v>
-      </c>
-      <c r="G79" t="n">
-        <v>1.59166666666667</v>
       </c>
     </row>
     <row r="80">
@@ -7207,16 +7207,16 @@
         <v>1.5</v>
       </c>
       <c r="D80" t="n">
+        <v>1.71666666666667</v>
+      </c>
+      <c r="E80" t="n">
         <v>0.216666666666667</v>
       </c>
-      <c r="E80" t="n">
-        <v>1.71666666666667</v>
-      </c>
       <c r="F80" t="n">
+        <v>2.04166666666667</v>
+      </c>
+      <c r="G80" t="n">
         <v>0.541666666666667</v>
-      </c>
-      <c r="G80" t="n">
-        <v>2.04166666666667</v>
       </c>
     </row>
     <row r="81">
@@ -7230,16 +7230,16 @@
         <v>1.4</v>
       </c>
       <c r="D81" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E81" t="n">
         <v>0.0999999999999999</v>
       </c>
-      <c r="E81" t="n">
-        <v>1.5</v>
-      </c>
       <c r="F81" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="G81" t="n">
         <v>0.116666666666666</v>
-      </c>
-      <c r="G81" t="n">
-        <v>1.51666666666667</v>
       </c>
     </row>
     <row r="82">
@@ -7253,16 +7253,16 @@
         <v>1.65</v>
       </c>
       <c r="D82" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="E82" t="n">
         <v>-0.0250000000000001</v>
       </c>
-      <c r="E82" t="n">
-        <v>1.625</v>
-      </c>
       <c r="F82" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="G82" t="n">
         <v>0.00833333333333308</v>
-      </c>
-      <c r="G82" t="n">
-        <v>1.65833333333333</v>
       </c>
     </row>
     <row r="83">
@@ -7276,10 +7276,10 @@
         <v>1.675</v>
       </c>
       <c r="D83" t="n">
+        <v>2.13333333333333</v>
+      </c>
+      <c r="E83" t="n">
         <v>0.458333333333333</v>
-      </c>
-      <c r="E83" t="n">
-        <v>2.13333333333333</v>
       </c>
       <c r="F83"/>
       <c r="G83"/>
@@ -7295,16 +7295,16 @@
         <v>1.525</v>
       </c>
       <c r="D84" t="n">
+        <v>1.91666666666667</v>
+      </c>
+      <c r="E84" t="n">
         <v>0.391666666666667</v>
       </c>
-      <c r="E84" t="n">
-        <v>1.91666666666667</v>
-      </c>
       <c r="F84" t="n">
+        <v>2</v>
+      </c>
+      <c r="G84" t="n">
         <v>0.475</v>
-      </c>
-      <c r="G84" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -7318,10 +7318,10 @@
         <v>1.5</v>
       </c>
       <c r="D85" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="E85" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="E85" t="n">
-        <v>1.60833333333333</v>
       </c>
       <c r="F85"/>
       <c r="G85"/>
@@ -7337,16 +7337,16 @@
         <v>1.28333333333333</v>
       </c>
       <c r="D86" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="E86" t="n">
         <v>0.15</v>
       </c>
-      <c r="E86" t="n">
-        <v>1.43333333333333</v>
-      </c>
       <c r="F86" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="G86" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G86" t="n">
-        <v>1.44166666666667</v>
       </c>
     </row>
     <row r="87">
@@ -7360,16 +7360,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D87" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="E87" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E87" t="n">
-        <v>1.61666666666667</v>
-      </c>
       <c r="F87" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="G87" t="n">
         <v>0.141666666666667</v>
-      </c>
-      <c r="G87" t="n">
-        <v>1.65</v>
       </c>
     </row>
     <row r="88">
@@ -7383,16 +7383,16 @@
         <v>1.56666666666667</v>
       </c>
       <c r="D88" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="E88" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E88" t="n">
-        <v>1.60833333333333</v>
-      </c>
       <c r="F88" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="G88" t="n">
         <v>0.0499999999999998</v>
-      </c>
-      <c r="G88" t="n">
-        <v>1.61666666666667</v>
       </c>
     </row>
     <row r="89">
@@ -7406,16 +7406,16 @@
         <v>1.49166666666667</v>
       </c>
       <c r="D89" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="E89" t="n">
         <v>0.15</v>
       </c>
-      <c r="E89" t="n">
-        <v>1.64166666666667</v>
-      </c>
       <c r="F89" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="G89" t="n">
         <v>0.183333333333334</v>
-      </c>
-      <c r="G89" t="n">
-        <v>1.675</v>
       </c>
     </row>
     <row r="90">
@@ -7429,16 +7429,16 @@
         <v>1.65</v>
       </c>
       <c r="D90" t="n">
+        <v>1.725</v>
+      </c>
+      <c r="E90" t="n">
         <v>0.0750000000000002</v>
       </c>
-      <c r="E90" t="n">
-        <v>1.725</v>
-      </c>
       <c r="F90" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G90" t="n">
         <v>0.0999999999999999</v>
-      </c>
-      <c r="G90" t="n">
-        <v>1.75</v>
       </c>
     </row>
     <row r="91">
@@ -7452,16 +7452,16 @@
         <v>1.34166666666667</v>
       </c>
       <c r="D91" t="n">
+        <v>1.38333333333333</v>
+      </c>
+      <c r="E91" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E91" t="n">
-        <v>1.38333333333333</v>
-      </c>
       <c r="F91" t="n">
+        <v>1.39166666666667</v>
+      </c>
+      <c r="G91" t="n">
         <v>0.0499999999999998</v>
-      </c>
-      <c r="G91" t="n">
-        <v>1.39166666666667</v>
       </c>
     </row>
     <row r="92">
@@ -7475,16 +7475,16 @@
         <v>1.43333333333333</v>
       </c>
       <c r="D92" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="E92" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="E92" t="n">
-        <v>1.51666666666667</v>
-      </c>
       <c r="F92" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="G92" t="n">
         <v>0.0916666666666668</v>
-      </c>
-      <c r="G92" t="n">
-        <v>1.525</v>
       </c>
     </row>
     <row r="93">
@@ -7498,16 +7498,16 @@
         <v>1.63333333333333</v>
       </c>
       <c r="D93" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="E93" t="n">
         <v>0.00833333333333308</v>
       </c>
-      <c r="E93" t="n">
-        <v>1.64166666666667</v>
-      </c>
       <c r="F93" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="G93" t="n">
         <v>0.0166666666666666</v>
-      </c>
-      <c r="G93" t="n">
-        <v>1.65</v>
       </c>
     </row>
     <row r="94">
@@ -7521,16 +7521,16 @@
         <v>1.325</v>
       </c>
       <c r="D94" t="n">
+        <v>1.41666666666667</v>
+      </c>
+      <c r="E94" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E94" t="n">
-        <v>1.41666666666667</v>
-      </c>
       <c r="F94" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="G94" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G94" t="n">
-        <v>1.43333333333333</v>
       </c>
     </row>
     <row r="95">
@@ -7544,16 +7544,16 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D95" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E95" t="n">
         <v>0.158333333333333</v>
       </c>
-      <c r="E95" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F95" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="G95" t="n">
         <v>0.175</v>
-      </c>
-      <c r="G95" t="n">
-        <v>1.61666666666667</v>
       </c>
     </row>
     <row r="96">
@@ -7567,16 +7567,16 @@
         <v>1.33333333333333</v>
       </c>
       <c r="D96" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="E96" t="n">
         <v>0.1</v>
       </c>
-      <c r="E96" t="n">
-        <v>1.43333333333333</v>
-      </c>
       <c r="F96" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="G96" t="n">
         <v>0.116666666666667</v>
-      </c>
-      <c r="G96" t="n">
-        <v>1.45</v>
       </c>
     </row>
     <row r="97">
@@ -7590,16 +7590,16 @@
         <v>1.275</v>
       </c>
       <c r="D97" t="n">
+        <v>1.34166666666667</v>
+      </c>
+      <c r="E97" t="n">
         <v>0.0666666666666667</v>
       </c>
-      <c r="E97" t="n">
+      <c r="F97" t="n">
         <v>1.34166666666667</v>
       </c>
-      <c r="F97" t="n">
+      <c r="G97" t="n">
         <v>0.0666666666666667</v>
-      </c>
-      <c r="G97" t="n">
-        <v>1.34166666666667</v>
       </c>
     </row>
     <row r="98">
@@ -7613,16 +7613,16 @@
         <v>1.45833333333333</v>
       </c>
       <c r="D98" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="E98" t="n">
         <v>0.216666666666667</v>
       </c>
-      <c r="E98" t="n">
-        <v>1.675</v>
-      </c>
       <c r="F98" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G98" t="n">
         <v>0.241666666666667</v>
-      </c>
-      <c r="G98" t="n">
-        <v>1.7</v>
       </c>
     </row>
     <row r="99">
@@ -7636,16 +7636,16 @@
         <v>1.43333333333333</v>
       </c>
       <c r="D99" t="n">
+        <v>1.56666666666667</v>
+      </c>
+      <c r="E99" t="n">
         <v>0.133333333333333</v>
       </c>
-      <c r="E99" t="n">
-        <v>1.56666666666667</v>
-      </c>
       <c r="F99" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="G99" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G99" t="n">
-        <v>1.58333333333333</v>
       </c>
     </row>
     <row r="100">
@@ -7659,16 +7659,16 @@
         <v>1.49166666666667</v>
       </c>
       <c r="D100" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E100" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E100" t="n">
-        <v>1.63333333333333</v>
-      </c>
       <c r="F100" t="n">
+        <v>1.71666666666667</v>
+      </c>
+      <c r="G100" t="n">
         <v>0.225</v>
-      </c>
-      <c r="G100" t="n">
-        <v>1.71666666666667</v>
       </c>
     </row>
     <row r="101">
@@ -7682,16 +7682,16 @@
         <v>1.66666666666667</v>
       </c>
       <c r="D101" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="E101" t="n">
         <v>-0.0166666666666666</v>
       </c>
-      <c r="E101" t="n">
-        <v>1.65</v>
-      </c>
       <c r="F101" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="G101" t="n">
         <v>-0.00833333333333353</v>
-      </c>
-      <c r="G101" t="n">
-        <v>1.65833333333333</v>
       </c>
     </row>
     <row r="102">
@@ -7705,16 +7705,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D102" t="n">
+        <v>1.66666666666667</v>
+      </c>
+      <c r="E102" t="n">
         <v>0.158333333333333</v>
       </c>
-      <c r="E102" t="n">
-        <v>1.66666666666667</v>
-      </c>
       <c r="F102" t="n">
+        <v>1.70833333333333</v>
+      </c>
+      <c r="G102" t="n">
         <v>0.2</v>
-      </c>
-      <c r="G102" t="n">
-        <v>1.70833333333333</v>
       </c>
     </row>
     <row r="103">
@@ -7728,16 +7728,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D103" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="E103" t="n">
         <v>0.0416666666666665</v>
       </c>
-      <c r="E103" t="n">
-        <v>1.55</v>
-      </c>
       <c r="F103" t="n">
+        <v>1.56666666666667</v>
+      </c>
+      <c r="G103" t="n">
         <v>0.0583333333333331</v>
-      </c>
-      <c r="G103" t="n">
-        <v>1.56666666666667</v>
       </c>
     </row>
     <row r="104">
@@ -7751,16 +7751,16 @@
         <v>1.34166666666667</v>
       </c>
       <c r="D104" t="n">
+        <v>1.40833333333333</v>
+      </c>
+      <c r="E104" t="n">
         <v>0.0666666666666664</v>
       </c>
-      <c r="E104" t="n">
-        <v>1.40833333333333</v>
-      </c>
       <c r="F104" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="G104" t="n">
         <v>0.0833333333333333</v>
-      </c>
-      <c r="G104" t="n">
-        <v>1.425</v>
       </c>
     </row>
     <row r="105">
@@ -7774,16 +7774,16 @@
         <v>1.35833333333333</v>
       </c>
       <c r="D105" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="E105" t="n">
         <v>0.0999999999999999</v>
       </c>
-      <c r="E105" t="n">
-        <v>1.45833333333333</v>
-      </c>
       <c r="F105" t="n">
+        <v>1.48333333333333</v>
+      </c>
+      <c r="G105" t="n">
         <v>0.125</v>
-      </c>
-      <c r="G105" t="n">
-        <v>1.48333333333333</v>
       </c>
     </row>
     <row r="106">
@@ -7797,16 +7797,16 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D106" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E106" t="n">
         <v>0.1</v>
       </c>
-      <c r="E106" t="n">
-        <v>1.54166666666667</v>
-      </c>
       <c r="F106" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="G106" t="n">
         <v>0.133333333333333</v>
-      </c>
-      <c r="G106" t="n">
-        <v>1.575</v>
       </c>
     </row>
     <row r="107">
@@ -7820,16 +7820,16 @@
         <v>1.40833333333333</v>
       </c>
       <c r="D107" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="E107" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E107" t="n">
-        <v>1.55</v>
-      </c>
       <c r="F107" t="n">
+        <v>1.56666666666667</v>
+      </c>
+      <c r="G107" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G107" t="n">
-        <v>1.56666666666667</v>
       </c>
     </row>
     <row r="108">
@@ -7843,16 +7843,16 @@
         <v>1.3</v>
       </c>
       <c r="D108" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="E108" t="n">
         <v>0.225</v>
       </c>
-      <c r="E108" t="n">
-        <v>1.525</v>
-      </c>
       <c r="F108" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="G108" t="n">
         <v>0.25</v>
-      </c>
-      <c r="G108" t="n">
-        <v>1.55</v>
       </c>
     </row>
     <row r="109">
@@ -7866,16 +7866,16 @@
         <v>1.6</v>
       </c>
       <c r="D109" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E109" t="n">
         <v>-0.00833333333333308</v>
       </c>
-      <c r="E109" t="n">
-        <v>1.59166666666667</v>
-      </c>
       <c r="F109" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="G109" t="n">
         <v>0.0333333333333337</v>
-      </c>
-      <c r="G109" t="n">
-        <v>1.63333333333333</v>
       </c>
     </row>
     <row r="110">
@@ -7889,16 +7889,16 @@
         <v>1.53333333333333</v>
       </c>
       <c r="D110" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="E110" t="n">
         <v>0</v>
       </c>
-      <c r="E110" t="n">
-        <v>1.53333333333333</v>
-      </c>
       <c r="F110" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="G110" t="n">
         <v>0.00833333333333353</v>
-      </c>
-      <c r="G110" t="n">
-        <v>1.54166666666667</v>
       </c>
     </row>
     <row r="111">
@@ -7912,16 +7912,16 @@
         <v>1.54166666666667</v>
       </c>
       <c r="D111" t="n">
+        <v>1.73333333333333</v>
+      </c>
+      <c r="E111" t="n">
         <v>0.191666666666667</v>
       </c>
-      <c r="E111" t="n">
-        <v>1.73333333333333</v>
-      </c>
       <c r="F111" t="n">
+        <v>1.66666666666667</v>
+      </c>
+      <c r="G111" t="n">
         <v>0.125</v>
-      </c>
-      <c r="G111" t="n">
-        <v>1.66666666666667</v>
       </c>
     </row>
     <row r="112">
@@ -7935,16 +7935,16 @@
         <v>1.375</v>
       </c>
       <c r="D112" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E112" t="n">
         <v>0.075</v>
       </c>
-      <c r="E112" t="n">
-        <v>1.45</v>
-      </c>
       <c r="F112" t="n">
+        <v>1.475</v>
+      </c>
+      <c r="G112" t="n">
         <v>0.0999999999999999</v>
-      </c>
-      <c r="G112" t="n">
-        <v>1.475</v>
       </c>
     </row>
     <row r="113">
@@ -7958,16 +7958,16 @@
         <v>1.39166666666667</v>
       </c>
       <c r="D113" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E113" t="n">
         <v>0.2</v>
       </c>
-      <c r="E113" t="n">
-        <v>1.59166666666667</v>
-      </c>
       <c r="F113" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="G113" t="n">
         <v>0.216666666666667</v>
-      </c>
-      <c r="G113" t="n">
-        <v>1.60833333333333</v>
       </c>
     </row>
     <row r="114">
@@ -7981,16 +7981,16 @@
         <v>1.3</v>
       </c>
       <c r="D114" t="n">
+        <v>1.41666666666667</v>
+      </c>
+      <c r="E114" t="n">
         <v>0.116666666666667</v>
       </c>
-      <c r="E114" t="n">
+      <c r="F114" t="n">
         <v>1.41666666666667</v>
       </c>
-      <c r="F114" t="n">
+      <c r="G114" t="n">
         <v>0.116666666666667</v>
-      </c>
-      <c r="G114" t="n">
-        <v>1.41666666666667</v>
       </c>
     </row>
     <row r="115">
@@ -8004,16 +8004,16 @@
         <v>1.34166666666667</v>
       </c>
       <c r="D115" t="n">
+        <v>1.41666666666667</v>
+      </c>
+      <c r="E115" t="n">
         <v>0.075</v>
       </c>
-      <c r="E115" t="n">
-        <v>1.41666666666667</v>
-      </c>
       <c r="F115" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="G115" t="n">
         <v>0.0916666666666666</v>
-      </c>
-      <c r="G115" t="n">
-        <v>1.43333333333333</v>
       </c>
     </row>
     <row r="116">
@@ -8027,16 +8027,16 @@
         <v>1.35</v>
       </c>
       <c r="D116" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E116" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E116" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F116" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="G116" t="n">
         <v>0.175</v>
-      </c>
-      <c r="G116" t="n">
-        <v>1.525</v>
       </c>
     </row>
     <row r="117">
@@ -8050,16 +8050,16 @@
         <v>1.35833333333333</v>
       </c>
       <c r="D117" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="E117" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="E117" t="n">
-        <v>1.44166666666667</v>
-      </c>
       <c r="F117" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="G117" t="n">
         <v>0.0916666666666666</v>
-      </c>
-      <c r="G117" t="n">
-        <v>1.45</v>
       </c>
     </row>
     <row r="118">
@@ -8073,16 +8073,16 @@
         <v>1.425</v>
       </c>
       <c r="D118" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="E118" t="n">
         <v>0.0916666666666666</v>
       </c>
-      <c r="E118" t="n">
-        <v>1.51666666666667</v>
-      </c>
       <c r="F118" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="G118" t="n">
         <v>0.1</v>
-      </c>
-      <c r="G118" t="n">
-        <v>1.525</v>
       </c>
     </row>
     <row r="119">
@@ -8096,16 +8096,16 @@
         <v>1.46666666666667</v>
       </c>
       <c r="D119" t="n">
+        <v>1.56666666666667</v>
+      </c>
+      <c r="E119" t="n">
         <v>0.0999999999999999</v>
       </c>
-      <c r="E119" t="n">
-        <v>1.56666666666667</v>
-      </c>
       <c r="F119" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="G119" t="n">
         <v>0.0583333333333333</v>
-      </c>
-      <c r="G119" t="n">
-        <v>1.525</v>
       </c>
     </row>
     <row r="120">
@@ -8119,16 +8119,16 @@
         <v>1.46666666666667</v>
       </c>
       <c r="D120" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E120" t="n">
         <v>0.125</v>
       </c>
-      <c r="E120" t="n">
-        <v>1.59166666666667</v>
-      </c>
       <c r="F120" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G120" t="n">
         <v>0.133333333333333</v>
-      </c>
-      <c r="G120" t="n">
-        <v>1.6</v>
       </c>
     </row>
     <row r="121">
@@ -8142,16 +8142,16 @@
         <v>1.51666666666667</v>
       </c>
       <c r="D121" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E121" t="n">
         <v>0.0250000000000001</v>
       </c>
-      <c r="E121" t="n">
+      <c r="F121" t="n">
         <v>1.54166666666667</v>
       </c>
-      <c r="F121" t="n">
+      <c r="G121" t="n">
         <v>0.0250000000000001</v>
-      </c>
-      <c r="G121" t="n">
-        <v>1.54166666666667</v>
       </c>
     </row>
     <row r="122">
@@ -8165,16 +8165,16 @@
         <v>1.40833333333333</v>
       </c>
       <c r="D122" t="n">
+        <v>1.55833333333333</v>
+      </c>
+      <c r="E122" t="n">
         <v>0.15</v>
       </c>
-      <c r="E122" t="n">
-        <v>1.55833333333333</v>
-      </c>
       <c r="F122" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="G122" t="n">
         <v>0.175</v>
-      </c>
-      <c r="G122" t="n">
-        <v>1.58333333333333</v>
       </c>
     </row>
     <row r="123">
@@ -8188,16 +8188,16 @@
         <v>1.60833333333333</v>
       </c>
       <c r="D123" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="E123" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E123" t="n">
-        <v>1.75</v>
-      </c>
       <c r="F123" t="n">
+        <v>1.75833333333333</v>
+      </c>
+      <c r="G123" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G123" t="n">
-        <v>1.75833333333333</v>
       </c>
     </row>
     <row r="124">
@@ -8211,16 +8211,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D124" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="E124" t="n">
         <v>-0.0500000000000003</v>
       </c>
-      <c r="E124" t="n">
+      <c r="F124" t="n">
         <v>1.45833333333333</v>
       </c>
-      <c r="F124" t="n">
+      <c r="G124" t="n">
         <v>-0.0500000000000003</v>
-      </c>
-      <c r="G124" t="n">
-        <v>1.45833333333333</v>
       </c>
     </row>
     <row r="125">
@@ -8234,16 +8234,16 @@
         <v>1.35833333333333</v>
       </c>
       <c r="D125" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E125" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E125" t="n">
-        <v>1.5</v>
-      </c>
       <c r="F125" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="G125" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G125" t="n">
-        <v>1.51666666666667</v>
       </c>
     </row>
     <row r="126">
@@ -8257,16 +8257,16 @@
         <v>1.36666666666667</v>
       </c>
       <c r="D126" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E126" t="n">
         <v>0.133333333333334</v>
       </c>
-      <c r="E126" t="n">
-        <v>1.5</v>
-      </c>
       <c r="F126" t="n">
+        <v>1.50833333333333</v>
+      </c>
+      <c r="G126" t="n">
         <v>0.141666666666667</v>
-      </c>
-      <c r="G126" t="n">
-        <v>1.50833333333333</v>
       </c>
     </row>
     <row r="127">
@@ -8280,10 +8280,10 @@
         <v>1.625</v>
       </c>
       <c r="D127" t="n">
+        <v>2.025</v>
+      </c>
+      <c r="E127" t="n">
         <v>0.4</v>
-      </c>
-      <c r="E127" t="n">
-        <v>2.025</v>
       </c>
       <c r="F127"/>
       <c r="G127"/>
@@ -8299,10 +8299,10 @@
         <v>1.6</v>
       </c>
       <c r="D128" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="E128" t="n">
         <v>0.0416666666666667</v>
-      </c>
-      <c r="E128" t="n">
-        <v>1.64166666666667</v>
       </c>
       <c r="F128"/>
       <c r="G128"/>
@@ -8318,16 +8318,16 @@
         <v>1.34166666666667</v>
       </c>
       <c r="D129" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E129" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E129" t="n">
-        <v>1.45</v>
-      </c>
       <c r="F129" t="n">
+        <v>1.46666666666667</v>
+      </c>
+      <c r="G129" t="n">
         <v>0.125</v>
-      </c>
-      <c r="G129" t="n">
-        <v>1.46666666666667</v>
       </c>
     </row>
     <row r="130">
@@ -8341,16 +8341,16 @@
         <v>1.55833333333333</v>
       </c>
       <c r="D130" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E130" t="n">
         <v>0.0750000000000002</v>
       </c>
-      <c r="E130" t="n">
-        <v>1.63333333333333</v>
-      </c>
       <c r="F130" t="n">
+        <v>1.69166666666667</v>
+      </c>
+      <c r="G130" t="n">
         <v>0.133333333333333</v>
-      </c>
-      <c r="G130" t="n">
-        <v>1.69166666666667</v>
       </c>
     </row>
     <row r="131">
@@ -8364,16 +8364,16 @@
         <v>1.33333333333333</v>
       </c>
       <c r="D131" t="n">
+        <v>1.46666666666667</v>
+      </c>
+      <c r="E131" t="n">
         <v>0.133333333333334</v>
       </c>
-      <c r="E131" t="n">
-        <v>1.46666666666667</v>
-      </c>
       <c r="F131" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="G131" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G131" t="n">
-        <v>1.49166666666667</v>
       </c>
     </row>
     <row r="132">
@@ -8387,16 +8387,16 @@
         <v>1.25833333333333</v>
       </c>
       <c r="D132" t="n">
+        <v>1.48333333333333</v>
+      </c>
+      <c r="E132" t="n">
         <v>0.225</v>
       </c>
-      <c r="E132" t="n">
-        <v>1.48333333333333</v>
-      </c>
       <c r="F132" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="G132" t="n">
         <v>0.233333333333333</v>
-      </c>
-      <c r="G132" t="n">
-        <v>1.49166666666667</v>
       </c>
     </row>
     <row r="133">
@@ -8410,16 +8410,16 @@
         <v>1.41666666666667</v>
       </c>
       <c r="D133" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="E133" t="n">
         <v>0.208333333333333</v>
       </c>
-      <c r="E133" t="n">
-        <v>1.625</v>
-      </c>
       <c r="F133" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="G133" t="n">
         <v>0.241666666666666</v>
-      </c>
-      <c r="G133" t="n">
-        <v>1.65833333333333</v>
       </c>
     </row>
     <row r="134">
@@ -8433,16 +8433,16 @@
         <v>1.275</v>
       </c>
       <c r="D134" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E134" t="n">
         <v>0.0749999999999997</v>
       </c>
-      <c r="E134" t="n">
-        <v>1.35</v>
-      </c>
       <c r="F134" t="n">
+        <v>1.35833333333333</v>
+      </c>
+      <c r="G134" t="n">
         <v>0.0833333333333333</v>
-      </c>
-      <c r="G134" t="n">
-        <v>1.35833333333333</v>
       </c>
     </row>
     <row r="135">
@@ -8456,16 +8456,16 @@
         <v>1.575</v>
       </c>
       <c r="D135" t="n">
+        <v>1.55833333333333</v>
+      </c>
+      <c r="E135" t="n">
         <v>-0.0166666666666666</v>
       </c>
-      <c r="E135" t="n">
-        <v>1.55833333333333</v>
-      </c>
       <c r="F135" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="G135" t="n">
         <v>0.0083333333333333</v>
-      </c>
-      <c r="G135" t="n">
-        <v>1.58333333333333</v>
       </c>
     </row>
     <row r="136">
@@ -8479,16 +8479,16 @@
         <v>1.48333333333333</v>
       </c>
       <c r="D136" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E136" t="n">
         <v>0.15</v>
       </c>
-      <c r="E136" t="n">
+      <c r="F136" t="n">
         <v>1.63333333333333</v>
       </c>
-      <c r="F136" t="n">
+      <c r="G136" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G136" t="n">
-        <v>1.63333333333333</v>
       </c>
     </row>
     <row r="137">
@@ -8502,16 +8502,16 @@
         <v>1.58333333333333</v>
       </c>
       <c r="D137" t="n">
+        <v>1.70833333333333</v>
+      </c>
+      <c r="E137" t="n">
         <v>0.125</v>
       </c>
-      <c r="E137" t="n">
-        <v>1.70833333333333</v>
-      </c>
       <c r="F137" t="n">
+        <v>1.74166666666667</v>
+      </c>
+      <c r="G137" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G137" t="n">
-        <v>1.74166666666667</v>
       </c>
     </row>
     <row r="138">
@@ -8525,16 +8525,16 @@
         <v>1.325</v>
       </c>
       <c r="D138" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="E138" t="n">
         <v>0.116666666666667</v>
       </c>
-      <c r="E138" t="n">
-        <v>1.44166666666667</v>
-      </c>
       <c r="F138" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="G138" t="n">
         <v>0.133333333333333</v>
-      </c>
-      <c r="G138" t="n">
-        <v>1.45833333333333</v>
       </c>
     </row>
     <row r="139">
@@ -8548,16 +8548,16 @@
         <v>1.39166666666667</v>
       </c>
       <c r="D139" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E139" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E139" t="n">
-        <v>1.5</v>
-      </c>
       <c r="F139" t="n">
+        <v>1.50833333333333</v>
+      </c>
+      <c r="G139" t="n">
         <v>0.116666666666667</v>
-      </c>
-      <c r="G139" t="n">
-        <v>1.50833333333333</v>
       </c>
     </row>
     <row r="140">
@@ -8571,10 +8571,10 @@
         <v>1.40833333333333</v>
       </c>
       <c r="D140" t="n">
+        <v>1.475</v>
+      </c>
+      <c r="E140" t="n">
         <v>0.0666666666666667</v>
-      </c>
-      <c r="E140" t="n">
-        <v>1.475</v>
       </c>
       <c r="F140"/>
       <c r="G140"/>
@@ -8590,16 +8590,16 @@
         <v>1.45</v>
       </c>
       <c r="D141" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E141" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E141" t="n">
-        <v>1.54166666666667</v>
-      </c>
       <c r="F141" t="n">
+        <v>1.55833333333333</v>
+      </c>
+      <c r="G141" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G141" t="n">
-        <v>1.55833333333333</v>
       </c>
     </row>
     <row r="142">
@@ -8613,10 +8613,10 @@
         <v>1.51666666666667</v>
       </c>
       <c r="D142" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="E142" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="E142" t="n">
-        <v>1.675</v>
       </c>
       <c r="F142"/>
       <c r="G142"/>
@@ -8632,16 +8632,16 @@
         <v>1.5</v>
       </c>
       <c r="D143" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E143" t="n">
         <v>0.075</v>
       </c>
-      <c r="E143" t="n">
-        <v>1.575</v>
-      </c>
       <c r="F143" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="G143" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G143" t="n">
-        <v>1.60833333333333</v>
       </c>
     </row>
     <row r="144">
@@ -8655,16 +8655,16 @@
         <v>1.45</v>
       </c>
       <c r="D144" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="E144" t="n">
         <v>0.1</v>
       </c>
-      <c r="E144" t="n">
-        <v>1.55</v>
-      </c>
       <c r="F144" t="n">
+        <v>1.56666666666667</v>
+      </c>
+      <c r="G144" t="n">
         <v>0.116666666666667</v>
-      </c>
-      <c r="G144" t="n">
-        <v>1.56666666666667</v>
       </c>
     </row>
     <row r="145">
@@ -8678,16 +8678,16 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D145" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E145" t="n">
         <v>0.0499999999999998</v>
       </c>
-      <c r="E145" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F145" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="G145" t="n">
         <v>0.075</v>
-      </c>
-      <c r="G145" t="n">
-        <v>1.51666666666667</v>
       </c>
     </row>
     <row r="146">
@@ -8701,16 +8701,16 @@
         <v>1.65833333333333</v>
       </c>
       <c r="D146" t="n">
+        <v>1.61666666666667</v>
+      </c>
+      <c r="E146" t="n">
         <v>-0.0416666666666667</v>
       </c>
-      <c r="E146" t="n">
-        <v>1.61666666666667</v>
-      </c>
       <c r="F146" t="n">
+        <v>1.68333333333333</v>
+      </c>
+      <c r="G146" t="n">
         <v>0.0250000000000004</v>
-      </c>
-      <c r="G146" t="n">
-        <v>1.68333333333333</v>
       </c>
     </row>
     <row r="147">
@@ -8724,16 +8724,16 @@
         <v>1.35833333333333</v>
       </c>
       <c r="D147" t="n">
+        <v>1.46666666666667</v>
+      </c>
+      <c r="E147" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E147" t="n">
+      <c r="F147" t="n">
         <v>1.46666666666667</v>
       </c>
-      <c r="F147" t="n">
+      <c r="G147" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G147" t="n">
-        <v>1.46666666666667</v>
       </c>
     </row>
     <row r="148">
@@ -8747,10 +8747,10 @@
         <v>1.625</v>
       </c>
       <c r="D148" t="n">
+        <v>1.75833333333333</v>
+      </c>
+      <c r="E148" t="n">
         <v>0.133333333333334</v>
-      </c>
-      <c r="E148" t="n">
-        <v>1.75833333333333</v>
       </c>
       <c r="F148"/>
       <c r="G148"/>
@@ -8766,16 +8766,16 @@
         <v>1.34166666666667</v>
       </c>
       <c r="D149" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="E149" t="n">
         <v>0.0999999999999999</v>
       </c>
-      <c r="E149" t="n">
-        <v>1.44166666666667</v>
-      </c>
       <c r="F149" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="G149" t="n">
         <v>0.116666666666666</v>
-      </c>
-      <c r="G149" t="n">
-        <v>1.45833333333333</v>
       </c>
     </row>
     <row r="150">
@@ -8789,16 +8789,16 @@
         <v>1.58333333333333</v>
       </c>
       <c r="D150" t="n">
+        <v>1.76666666666667</v>
+      </c>
+      <c r="E150" t="n">
         <v>0.183333333333334</v>
       </c>
-      <c r="E150" t="n">
-        <v>1.76666666666667</v>
-      </c>
       <c r="F150" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G150" t="n">
         <v>0.166666666666667</v>
-      </c>
-      <c r="G150" t="n">
-        <v>1.75</v>
       </c>
     </row>
     <row r="151">
@@ -8812,10 +8812,10 @@
         <v>1.5</v>
       </c>
       <c r="D151" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E151" t="n">
         <v>0.0416666666666667</v>
-      </c>
-      <c r="E151" t="n">
-        <v>1.54166666666667</v>
       </c>
       <c r="F151"/>
       <c r="G151"/>
@@ -8831,16 +8831,16 @@
         <v>1.26666666666667</v>
       </c>
       <c r="D152" t="n">
+        <v>1.39166666666667</v>
+      </c>
+      <c r="E152" t="n">
         <v>0.125</v>
       </c>
-      <c r="E152" t="n">
-        <v>1.39166666666667</v>
-      </c>
       <c r="F152" t="n">
+        <v>1.40833333333333</v>
+      </c>
+      <c r="G152" t="n">
         <v>0.141666666666667</v>
-      </c>
-      <c r="G152" t="n">
-        <v>1.40833333333333</v>
       </c>
     </row>
     <row r="153">
@@ -8854,16 +8854,16 @@
         <v>1.40833333333333</v>
       </c>
       <c r="D153" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="E153" t="n">
         <v>0.183333333333334</v>
       </c>
-      <c r="E153" t="n">
-        <v>1.59166666666667</v>
-      </c>
       <c r="F153" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="G153" t="n">
         <v>0.225</v>
-      </c>
-      <c r="G153" t="n">
-        <v>1.63333333333333</v>
       </c>
     </row>
     <row r="154">
@@ -8877,16 +8877,16 @@
         <v>1.69166666666667</v>
       </c>
       <c r="D154" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="E154" t="n">
         <v>-0.05</v>
       </c>
-      <c r="E154" t="n">
-        <v>1.64166666666667</v>
-      </c>
       <c r="F154" t="n">
+        <v>1.65833333333333</v>
+      </c>
+      <c r="G154" t="n">
         <v>-0.0333333333333334</v>
-      </c>
-      <c r="G154" t="n">
-        <v>1.65833333333333</v>
       </c>
     </row>
     <row r="155">
@@ -8900,16 +8900,16 @@
         <v>1.45833333333333</v>
       </c>
       <c r="D155" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="E155" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E155" t="n">
-        <v>1.55</v>
-      </c>
       <c r="F155" t="n">
+        <v>1.56666666666667</v>
+      </c>
+      <c r="G155" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G155" t="n">
-        <v>1.56666666666667</v>
       </c>
     </row>
     <row r="156">
@@ -8923,16 +8923,16 @@
         <v>1.325</v>
       </c>
       <c r="D156" t="n">
+        <v>1.375</v>
+      </c>
+      <c r="E156" t="n">
         <v>0.05</v>
       </c>
-      <c r="E156" t="n">
-        <v>1.375</v>
-      </c>
       <c r="F156" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="G156" t="n">
         <v>0.0249999999999999</v>
-      </c>
-      <c r="G156" t="n">
-        <v>1.35</v>
       </c>
     </row>
     <row r="157">
@@ -8946,16 +8946,16 @@
         <v>1.30833333333333</v>
       </c>
       <c r="D157" t="n">
+        <v>1.48333333333333</v>
+      </c>
+      <c r="E157" t="n">
         <v>0.175</v>
       </c>
-      <c r="E157" t="n">
-        <v>1.48333333333333</v>
-      </c>
       <c r="F157" t="n">
+        <v>1.50833333333333</v>
+      </c>
+      <c r="G157" t="n">
         <v>0.2</v>
-      </c>
-      <c r="G157" t="n">
-        <v>1.50833333333333</v>
       </c>
     </row>
     <row r="158">
@@ -8969,16 +8969,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D158" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E158" t="n">
         <v>0.0666666666666664</v>
       </c>
-      <c r="E158" t="n">
-        <v>1.575</v>
-      </c>
       <c r="F158" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="G158" t="n">
         <v>0.0833333333333333</v>
-      </c>
-      <c r="G158" t="n">
-        <v>1.59166666666667</v>
       </c>
     </row>
     <row r="159">
@@ -8992,16 +8992,16 @@
         <v>1.38333333333333</v>
       </c>
       <c r="D159" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="E159" t="n">
         <v>0.0416666666666665</v>
       </c>
-      <c r="E159" t="n">
-        <v>1.425</v>
-      </c>
       <c r="F159" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="G159" t="n">
         <v>0.0583333333333331</v>
-      </c>
-      <c r="G159" t="n">
-        <v>1.44166666666667</v>
       </c>
     </row>
     <row r="160">
@@ -9015,16 +9015,16 @@
         <v>1.63333333333333</v>
       </c>
       <c r="D160" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="E160" t="n">
         <v>0.0416666666666665</v>
       </c>
-      <c r="E160" t="n">
-        <v>1.675</v>
-      </c>
       <c r="F160" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G160" t="n">
         <v>0.0666666666666664</v>
-      </c>
-      <c r="G160" t="n">
-        <v>1.7</v>
       </c>
     </row>
     <row r="161">
@@ -9038,16 +9038,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D161" t="n">
+        <v>1.58333333333333</v>
+      </c>
+      <c r="E161" t="n">
         <v>0.0749999999999997</v>
       </c>
-      <c r="E161" t="n">
-        <v>1.58333333333333</v>
-      </c>
       <c r="F161" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="G161" t="n">
         <v>0.116666666666666</v>
-      </c>
-      <c r="G161" t="n">
-        <v>1.625</v>
       </c>
     </row>
     <row r="162">
@@ -9061,16 +9061,16 @@
         <v>1.48333333333333</v>
       </c>
       <c r="D162" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="E162" t="n">
         <v>0.166666666666667</v>
       </c>
-      <c r="E162" t="n">
-        <v>1.65</v>
-      </c>
       <c r="F162" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G162" t="n">
         <v>0.216666666666667</v>
-      </c>
-      <c r="G162" t="n">
-        <v>1.7</v>
       </c>
     </row>
     <row r="163">
@@ -9084,16 +9084,16 @@
         <v>1.25833333333333</v>
       </c>
       <c r="D163" t="n">
+        <v>1.40833333333333</v>
+      </c>
+      <c r="E163" t="n">
         <v>0.15</v>
       </c>
-      <c r="E163" t="n">
-        <v>1.40833333333333</v>
-      </c>
       <c r="F163" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="G163" t="n">
         <v>0.166666666666667</v>
-      </c>
-      <c r="G163" t="n">
-        <v>1.425</v>
       </c>
     </row>
     <row r="164">
@@ -9107,16 +9107,16 @@
         <v>1.425</v>
       </c>
       <c r="D164" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="E164" t="n">
         <v>0.0083333333333333</v>
       </c>
-      <c r="E164" t="n">
-        <v>1.43333333333333</v>
-      </c>
       <c r="F164" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="G164" t="n">
         <v>0.0333333333333332</v>
-      </c>
-      <c r="G164" t="n">
-        <v>1.45833333333333</v>
       </c>
     </row>
     <row r="165">
@@ -9130,16 +9130,16 @@
         <v>1.35833333333333</v>
       </c>
       <c r="D165" t="n">
+        <v>1.46666666666667</v>
+      </c>
+      <c r="E165" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E165" t="n">
+      <c r="F165" t="n">
         <v>1.46666666666667</v>
       </c>
-      <c r="F165" t="n">
+      <c r="G165" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G165" t="n">
-        <v>1.46666666666667</v>
       </c>
     </row>
     <row r="166">
@@ -9153,16 +9153,16 @@
         <v>1.36666666666667</v>
       </c>
       <c r="D166" t="n">
+        <v>1.48333333333333</v>
+      </c>
+      <c r="E166" t="n">
         <v>0.116666666666667</v>
       </c>
-      <c r="E166" t="n">
-        <v>1.48333333333333</v>
-      </c>
       <c r="F166" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="G166" t="n">
         <v>0.125</v>
-      </c>
-      <c r="G166" t="n">
-        <v>1.49166666666667</v>
       </c>
     </row>
     <row r="167">
@@ -9176,16 +9176,16 @@
         <v>1.28333333333333</v>
       </c>
       <c r="D167" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="E167" t="n">
         <v>0.175</v>
       </c>
-      <c r="E167" t="n">
-        <v>1.45833333333333</v>
-      </c>
       <c r="F167" t="n">
+        <v>1.48333333333333</v>
+      </c>
+      <c r="G167" t="n">
         <v>0.2</v>
-      </c>
-      <c r="G167" t="n">
-        <v>1.48333333333333</v>
       </c>
     </row>
     <row r="168">
@@ -9199,16 +9199,16 @@
         <v>1.425</v>
       </c>
       <c r="D168" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="E168" t="n">
         <v>0.0333333333333332</v>
       </c>
-      <c r="E168" t="n">
-        <v>1.45833333333333</v>
-      </c>
       <c r="F168" t="n">
+        <v>1.475</v>
+      </c>
+      <c r="G168" t="n">
         <v>0.0499999999999998</v>
-      </c>
-      <c r="G168" t="n">
-        <v>1.475</v>
       </c>
     </row>
     <row r="169">
@@ -9222,16 +9222,16 @@
         <v>1.38333333333333</v>
       </c>
       <c r="D169" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="E169" t="n">
         <v>0.141666666666667</v>
       </c>
-      <c r="E169" t="n">
-        <v>1.525</v>
-      </c>
       <c r="F169" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="G169" t="n">
         <v>0.158333333333333</v>
-      </c>
-      <c r="G169" t="n">
-        <v>1.54166666666667</v>
       </c>
     </row>
     <row r="170">
@@ -9245,16 +9245,16 @@
         <v>1.325</v>
       </c>
       <c r="D170" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="E170" t="n">
         <v>0.108333333333333</v>
       </c>
-      <c r="E170" t="n">
+      <c r="F170" t="n">
         <v>1.43333333333333</v>
       </c>
-      <c r="F170" t="n">
+      <c r="G170" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G170" t="n">
-        <v>1.43333333333333</v>
       </c>
     </row>
     <row r="171">
@@ -9268,16 +9268,16 @@
         <v>1.51666666666667</v>
       </c>
       <c r="D171" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E171" t="n">
         <v>0.0250000000000001</v>
       </c>
-      <c r="E171" t="n">
+      <c r="F171" t="n">
         <v>1.54166666666667</v>
       </c>
-      <c r="F171" t="n">
+      <c r="G171" t="n">
         <v>0.0250000000000001</v>
-      </c>
-      <c r="G171" t="n">
-        <v>1.54166666666667</v>
       </c>
     </row>
     <row r="172">
@@ -9291,16 +9291,16 @@
         <v>1.25833333333333</v>
       </c>
       <c r="D172" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E172" t="n">
         <v>0.0916666666666666</v>
       </c>
-      <c r="E172" t="n">
+      <c r="F172" t="n">
         <v>1.35</v>
       </c>
-      <c r="F172" t="n">
+      <c r="G172" t="n">
         <v>0.0916666666666666</v>
-      </c>
-      <c r="G172" t="n">
-        <v>1.35</v>
       </c>
     </row>
     <row r="173">
@@ -9314,16 +9314,16 @@
         <v>1.41666666666667</v>
       </c>
       <c r="D173" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="E173" t="n">
         <v>0.0999999999999999</v>
       </c>
-      <c r="E173" t="n">
-        <v>1.51666666666667</v>
-      </c>
       <c r="F173" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="G173" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G173" t="n">
-        <v>1.525</v>
       </c>
     </row>
     <row r="174">
@@ -9337,16 +9337,16 @@
         <v>1.46666666666667</v>
       </c>
       <c r="D174" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="E174" t="n">
         <v>0.0499999999999998</v>
       </c>
-      <c r="E174" t="n">
-        <v>1.51666666666667</v>
-      </c>
       <c r="F174" t="n">
+        <v>1.53333333333333</v>
+      </c>
+      <c r="G174" t="n">
         <v>0.0666666666666664</v>
-      </c>
-      <c r="G174" t="n">
-        <v>1.53333333333333</v>
       </c>
     </row>
     <row r="175">
@@ -9360,16 +9360,16 @@
         <v>1.65</v>
       </c>
       <c r="D175" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="E175" t="n">
         <v>-0.0250000000000001</v>
       </c>
-      <c r="E175" t="n">
-        <v>1.625</v>
-      </c>
       <c r="F175" t="n">
+        <v>1.64166666666667</v>
+      </c>
+      <c r="G175" t="n">
         <v>-0.00833333333333353</v>
-      </c>
-      <c r="G175" t="n">
-        <v>1.64166666666667</v>
       </c>
     </row>
     <row r="176">
@@ -9383,16 +9383,16 @@
         <v>1.65833333333333</v>
       </c>
       <c r="D176" t="n">
+        <v>1.71666666666667</v>
+      </c>
+      <c r="E176" t="n">
         <v>0.0583333333333336</v>
       </c>
-      <c r="E176" t="n">
-        <v>1.71666666666667</v>
-      </c>
       <c r="F176" t="n">
+        <v>1.75833333333333</v>
+      </c>
+      <c r="G176" t="n">
         <v>0.1</v>
-      </c>
-      <c r="G176" t="n">
-        <v>1.75833333333333</v>
       </c>
     </row>
     <row r="177">
@@ -9406,10 +9406,10 @@
         <v>1.53333333333333</v>
       </c>
       <c r="D177" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="E177" t="n">
         <v>0.116666666666667</v>
-      </c>
-      <c r="E177" t="n">
-        <v>1.65</v>
       </c>
       <c r="F177"/>
       <c r="G177"/>
@@ -9425,10 +9425,10 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D178" t="n">
+        <v>1.68333333333333</v>
+      </c>
+      <c r="E178" t="n">
         <v>0.175</v>
-      </c>
-      <c r="E178" t="n">
-        <v>1.68333333333333</v>
       </c>
       <c r="F178"/>
       <c r="G178"/>
@@ -9444,10 +9444,10 @@
         <v>1.56666666666667</v>
       </c>
       <c r="D179" t="n">
+        <v>1.69166666666667</v>
+      </c>
+      <c r="E179" t="n">
         <v>0.125</v>
-      </c>
-      <c r="E179" t="n">
-        <v>1.69166666666667</v>
       </c>
       <c r="F179"/>
       <c r="G179"/>
@@ -9463,16 +9463,16 @@
         <v>1.60833333333333</v>
       </c>
       <c r="D180" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E180" t="n">
         <v>-0.0333333333333334</v>
       </c>
-      <c r="E180" t="n">
-        <v>1.575</v>
-      </c>
       <c r="F180" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="G180" t="n">
         <v>-0.0166666666666666</v>
-      </c>
-      <c r="G180" t="n">
-        <v>1.59166666666667</v>
       </c>
     </row>
     <row r="181">
@@ -9486,16 +9486,16 @@
         <v>1.49166666666667</v>
       </c>
       <c r="D181" t="n">
+        <v>1.575</v>
+      </c>
+      <c r="E181" t="n">
         <v>0.0833333333333335</v>
       </c>
-      <c r="E181" t="n">
-        <v>1.575</v>
-      </c>
       <c r="F181" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G181" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G181" t="n">
-        <v>1.6</v>
       </c>
     </row>
     <row r="182">
@@ -9509,16 +9509,16 @@
         <v>1.36666666666667</v>
       </c>
       <c r="D182" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="E182" t="n">
         <v>0.0666666666666669</v>
       </c>
-      <c r="E182" t="n">
+      <c r="F182" t="n">
         <v>1.43333333333333</v>
       </c>
-      <c r="F182" t="n">
+      <c r="G182" t="n">
         <v>0.0666666666666669</v>
-      </c>
-      <c r="G182" t="n">
-        <v>1.43333333333333</v>
       </c>
     </row>
     <row r="183">
@@ -9532,16 +9532,16 @@
         <v>1.34166666666667</v>
       </c>
       <c r="D183" t="n">
+        <v>1.44166666666667</v>
+      </c>
+      <c r="E183" t="n">
         <v>0.0999999999999999</v>
       </c>
-      <c r="E183" t="n">
-        <v>1.44166666666667</v>
-      </c>
       <c r="F183" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="G183" t="n">
         <v>0.108333333333333</v>
-      </c>
-      <c r="G183" t="n">
-        <v>1.45</v>
       </c>
     </row>
     <row r="184">
@@ -9555,16 +9555,16 @@
         <v>1.525</v>
       </c>
       <c r="D184" t="n">
+        <v>1.50833333333333</v>
+      </c>
+      <c r="E184" t="n">
         <v>-0.0166666666666666</v>
       </c>
-      <c r="E184" t="n">
-        <v>1.50833333333333</v>
-      </c>
       <c r="F184" t="n">
+        <v>1.51666666666667</v>
+      </c>
+      <c r="G184" t="n">
         <v>-0.00833333333333353</v>
-      </c>
-      <c r="G184" t="n">
-        <v>1.51666666666667</v>
       </c>
     </row>
     <row r="185">
@@ -9578,16 +9578,16 @@
         <v>1.59166666666667</v>
       </c>
       <c r="D185" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E185" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E185" t="n">
-        <v>1.63333333333333</v>
-      </c>
       <c r="F185" t="n">
+        <v>1.68333333333333</v>
+      </c>
+      <c r="G185" t="n">
         <v>0.0916666666666668</v>
-      </c>
-      <c r="G185" t="n">
-        <v>1.68333333333333</v>
       </c>
     </row>
     <row r="186">
@@ -9601,16 +9601,16 @@
         <v>1.48333333333333</v>
       </c>
       <c r="D186" t="n">
+        <v>1.68333333333333</v>
+      </c>
+      <c r="E186" t="n">
         <v>0.2</v>
       </c>
-      <c r="E186" t="n">
-        <v>1.68333333333333</v>
-      </c>
       <c r="F186" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G186" t="n">
         <v>0.216666666666667</v>
-      </c>
-      <c r="G186" t="n">
-        <v>1.7</v>
       </c>
     </row>
     <row r="187">
@@ -9624,16 +9624,16 @@
         <v>1.375</v>
       </c>
       <c r="D187" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E187" t="n">
         <v>0.116666666666666</v>
       </c>
-      <c r="E187" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F187" t="n">
+        <v>1.50833333333333</v>
+      </c>
+      <c r="G187" t="n">
         <v>0.133333333333334</v>
-      </c>
-      <c r="G187" t="n">
-        <v>1.50833333333333</v>
       </c>
     </row>
     <row r="188">
@@ -9647,16 +9647,16 @@
         <v>1.39166666666667</v>
       </c>
       <c r="D188" t="n">
+        <v>1.54166666666667</v>
+      </c>
+      <c r="E188" t="n">
         <v>0.15</v>
       </c>
-      <c r="E188" t="n">
-        <v>1.54166666666667</v>
-      </c>
       <c r="F188" t="n">
+        <v>1.59166666666667</v>
+      </c>
+      <c r="G188" t="n">
         <v>0.2</v>
-      </c>
-      <c r="G188" t="n">
-        <v>1.59166666666667</v>
       </c>
     </row>
     <row r="189">
@@ -9670,16 +9670,16 @@
         <v>1.53333333333333</v>
       </c>
       <c r="D189" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="E189" t="n">
         <v>0.0750000000000002</v>
       </c>
-      <c r="E189" t="n">
+      <c r="F189" t="n">
         <v>1.60833333333333</v>
       </c>
-      <c r="F189" t="n">
+      <c r="G189" t="n">
         <v>0.0750000000000002</v>
-      </c>
-      <c r="G189" t="n">
-        <v>1.60833333333333</v>
       </c>
     </row>
     <row r="190">
@@ -9693,16 +9693,16 @@
         <v>1.44166666666667</v>
       </c>
       <c r="D190" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="E190" t="n">
         <v>0.208333333333333</v>
       </c>
-      <c r="E190" t="n">
-        <v>1.65</v>
-      </c>
       <c r="F190" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="G190" t="n">
         <v>0.191666666666667</v>
-      </c>
-      <c r="G190" t="n">
-        <v>1.63333333333333</v>
       </c>
     </row>
     <row r="191">
@@ -9716,16 +9716,16 @@
         <v>1.59166666666667</v>
       </c>
       <c r="D191" t="n">
+        <v>1.74166666666667</v>
+      </c>
+      <c r="E191" t="n">
         <v>0.15</v>
       </c>
-      <c r="E191" t="n">
-        <v>1.74166666666667</v>
-      </c>
       <c r="F191" t="n">
+        <v>1.80833333333333</v>
+      </c>
+      <c r="G191" t="n">
         <v>0.216666666666667</v>
-      </c>
-      <c r="G191" t="n">
-        <v>1.80833333333333</v>
       </c>
     </row>
     <row r="192">
@@ -9739,16 +9739,16 @@
         <v>1.36666666666667</v>
       </c>
       <c r="D192" t="n">
+        <v>1.45833333333333</v>
+      </c>
+      <c r="E192" t="n">
         <v>0.0916666666666668</v>
       </c>
-      <c r="E192" t="n">
-        <v>1.45833333333333</v>
-      </c>
       <c r="F192" t="n">
+        <v>1.48333333333333</v>
+      </c>
+      <c r="G192" t="n">
         <v>0.116666666666667</v>
-      </c>
-      <c r="G192" t="n">
-        <v>1.48333333333333</v>
       </c>
     </row>
     <row r="193">
@@ -9762,16 +9762,16 @@
         <v>1.41666666666667</v>
       </c>
       <c r="D193" t="n">
+        <v>1.49166666666667</v>
+      </c>
+      <c r="E193" t="n">
         <v>0.0749999999999997</v>
       </c>
-      <c r="E193" t="n">
-        <v>1.49166666666667</v>
-      </c>
       <c r="F193" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G193" t="n">
         <v>0.0833333333333333</v>
-      </c>
-      <c r="G193" t="n">
-        <v>1.5</v>
       </c>
     </row>
     <row r="194">
@@ -9785,10 +9785,10 @@
         <v>1.325</v>
       </c>
       <c r="D194" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E194" t="n">
         <v>0.175</v>
-      </c>
-      <c r="E194" t="n">
-        <v>1.5</v>
       </c>
       <c r="F194"/>
       <c r="G194"/>
@@ -9804,16 +9804,16 @@
         <v>1.65</v>
       </c>
       <c r="D195" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="E195" t="n">
         <v>0.225</v>
       </c>
-      <c r="E195" t="n">
-        <v>1.875</v>
-      </c>
       <c r="F195" t="n">
+        <v>1.90833333333333</v>
+      </c>
+      <c r="G195" t="n">
         <v>0.258333333333333</v>
-      </c>
-      <c r="G195" t="n">
-        <v>1.90833333333333</v>
       </c>
     </row>
     <row r="196">
@@ -9827,16 +9827,16 @@
         <v>1.35</v>
       </c>
       <c r="D196" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E196" t="n">
         <v>0.15</v>
       </c>
-      <c r="E196" t="n">
+      <c r="F196" t="n">
         <v>1.5</v>
       </c>
-      <c r="F196" t="n">
+      <c r="G196" t="n">
         <v>0.15</v>
-      </c>
-      <c r="G196" t="n">
-        <v>1.5</v>
       </c>
     </row>
     <row r="197">
@@ -9850,16 +9850,16 @@
         <v>1.45</v>
       </c>
       <c r="D197" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E197" t="n">
         <v>0.25</v>
       </c>
-      <c r="E197" t="n">
-        <v>1.7</v>
-      </c>
       <c r="F197" t="n">
+        <v>1.80833333333333</v>
+      </c>
+      <c r="G197" t="n">
         <v>0.358333333333334</v>
-      </c>
-      <c r="G197" t="n">
-        <v>1.80833333333333</v>
       </c>
     </row>
     <row r="198">
@@ -9873,16 +9873,16 @@
         <v>1.50833333333333</v>
       </c>
       <c r="D198" t="n">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="E198" t="n">
         <v>0.125</v>
       </c>
-      <c r="E198" t="n">
-        <v>1.63333333333333</v>
-      </c>
       <c r="F198" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="G198" t="n">
         <v>0.141666666666667</v>
-      </c>
-      <c r="G198" t="n">
-        <v>1.65</v>
       </c>
     </row>
     <row r="199">
@@ -9896,16 +9896,16 @@
         <v>1.45</v>
       </c>
       <c r="D199" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E199" t="n">
         <v>0.15</v>
       </c>
-      <c r="E199" t="n">
-        <v>1.6</v>
-      </c>
       <c r="F199" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="G199" t="n">
         <v>0.175</v>
-      </c>
-      <c r="G199" t="n">
-        <v>1.625</v>
       </c>
     </row>
     <row r="200">
@@ -9919,16 +9919,16 @@
         <v>1.30833333333333</v>
       </c>
       <c r="D200" t="n">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="E200" t="n">
         <v>0.125</v>
       </c>
-      <c r="E200" t="n">
-        <v>1.43333333333333</v>
-      </c>
       <c r="F200" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="G200" t="n">
         <v>0.141666666666667</v>
-      </c>
-      <c r="G200" t="n">
-        <v>1.45</v>
       </c>
     </row>
     <row r="201">
@@ -9942,10 +9942,10 @@
         <v>1.475</v>
       </c>
       <c r="D201" t="n">
+        <v>1.68333333333333</v>
+      </c>
+      <c r="E201" t="n">
         <v>0.208333333333334</v>
-      </c>
-      <c r="E201" t="n">
-        <v>1.68333333333333</v>
       </c>
       <c r="F201"/>
       <c r="G201"/>
@@ -9961,16 +9961,16 @@
         <v>1.49166666666667</v>
       </c>
       <c r="D202" t="n">
+        <v>1.60833333333333</v>
+      </c>
+      <c r="E202" t="n">
         <v>0.116666666666667</v>
       </c>
-      <c r="E202" t="n">
+      <c r="F202" t="n">
         <v>1.60833333333333</v>
       </c>
-      <c r="F202" t="n">
+      <c r="G202" t="n">
         <v>0.116666666666667</v>
-      </c>
-      <c r="G202" t="n">
-        <v>1.60833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>